<commit_message>
Pre-release for SFRA Certification q4 2020
</commit_message>
<xml_diff>
--- a/test/acceptance/Automation_info/SFCC_WPG_CodeceptJS_Automation_Scenarios.xlsx
+++ b/test/acceptance/Automation_info/SFCC_WPG_CodeceptJS_Automation_Scenarios.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cbackup\WorldPay\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanraich\Documents\Automation\Automation_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79479C8-C7C0-4325-9F26-D7D5A14A8429}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{A5207258-7478-4C48-AB6B-0AB69EFB8D85}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290"/>
   </bookViews>
   <sheets>
-    <sheet name="Acceptance_Scenarios" sheetId="2" r:id="rId1"/>
+    <sheet name="MobileFirst" sheetId="4" r:id="rId1"/>
+    <sheet name="RefArch" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,38 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
-  <si>
-    <t>Guest User placing an order with:</t>
-  </si>
-  <si>
-    <t>Credit Card Direct Authorised Status</t>
-  </si>
-  <si>
-    <t>Credit Card Direct Error Status</t>
-  </si>
-  <si>
-    <t>Credit Card Direct 3D Authorised Status</t>
-  </si>
-  <si>
-    <t>Credit Card Direct 3DS2 Authentication Authorised Status</t>
-  </si>
-  <si>
-    <t>Credit Card Direct 3DS2 Frictionless Authorised Status</t>
-  </si>
-  <si>
-    <t>Direct Credit Card</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="47">
   <si>
     <t>APMs</t>
   </si>
   <si>
-    <t>CODECEPTJS ACCEPTANCE TEST SCENARIOS</t>
-  </si>
-  <si>
-    <t>Credit Card Direct 3D Refused Status</t>
-  </si>
-  <si>
     <t>ACH Pay | Authorised</t>
   </si>
   <si>
@@ -80,9 +53,6 @@
     <t>China Union Pay | Authorised &amp; Refused</t>
   </si>
   <si>
-    <t>eNets | Authorised &amp; Refused</t>
-  </si>
-  <si>
     <t>Giropay | Authorised &amp; Refused</t>
   </si>
   <si>
@@ -98,9 +68,6 @@
     <t>P24 | Authorised &amp; Refused</t>
   </si>
   <si>
-    <t>PayPal | Authorised</t>
-  </si>
-  <si>
     <t>Poli | Authorised &amp; Refused</t>
   </si>
   <si>
@@ -125,31 +92,94 @@
     <t>Klarna Pay Later | Authorised &amp; Refused</t>
   </si>
   <si>
-    <t>Saved Card</t>
-  </si>
-  <si>
-    <t>Registered_Direct_3DS2_Saved_Card</t>
-  </si>
-  <si>
-    <t>Registered_Redirect_Normal_Saved_Card</t>
-  </si>
-  <si>
-    <t>Credit Card Direct Refused Status</t>
-  </si>
-  <si>
-    <t>Credit Card Direct 3DS2 Authetication Refused Status</t>
-  </si>
-  <si>
-    <t>Credit Card Direct 3DS2 Frictioless Refused Status</t>
-  </si>
-  <si>
-    <t>Registered User placing an order with:</t>
+    <t>Folder Name: MobileFirst_DefaultUI</t>
+  </si>
+  <si>
+    <t>CreditCard_Direct</t>
+  </si>
+  <si>
+    <t>CreditCard_Redirect (HPP)</t>
+  </si>
+  <si>
+    <t>Guest checkout Normal Card Authorised flow</t>
+  </si>
+  <si>
+    <t>Guest checkout 3DS Card Authorised flow</t>
+  </si>
+  <si>
+    <t>Guest checkout 3DS2 Card Authorised flow</t>
+  </si>
+  <si>
+    <t>Guest checkout 3DS2 Frictionless Card Authorised flow</t>
+  </si>
+  <si>
+    <t>Guest checkout Normal Card Refused flow</t>
+  </si>
+  <si>
+    <t>Guest checkout Normal Card Error flow</t>
+  </si>
+  <si>
+    <t>Guest checkout 3DS Card Refused flow</t>
+  </si>
+  <si>
+    <t>Guest checkout 3DS2 Card Refused flow</t>
+  </si>
+  <si>
+    <t>Guest checkout 3DS2 Frictionless Card Refused flow</t>
+  </si>
+  <si>
+    <t>Klarna Slice It | Authorised &amp; Refused</t>
+  </si>
+  <si>
+    <t>PayPal | Authorised &amp; Refused</t>
+  </si>
+  <si>
+    <t>Direct Apms (Registered checkout)</t>
+  </si>
+  <si>
+    <t>Direct APMs (Guest checkout))</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Redirect APMs (Guest checkout))</t>
+  </si>
+  <si>
+    <t>Redirect Apms (Registered checkout)</t>
+  </si>
+  <si>
+    <t>IDEAL | Authorised &amp; Refused</t>
+  </si>
+  <si>
+    <t>Folder Name: RefArch_PluginUI</t>
+  </si>
+  <si>
+    <t>APMs_NUI</t>
+  </si>
+  <si>
+    <t>CreditCard_Direct_NUI</t>
+  </si>
+  <si>
+    <t>CreditCard_Redirect_NUI (HPP)</t>
+  </si>
+  <si>
+    <t>Direct APMs NUI (Guest checkout))</t>
+  </si>
+  <si>
+    <t>Direct Apms NUI (Registered checkout)</t>
+  </si>
+  <si>
+    <t>Redirect APMs NUI (Guest checkout))</t>
+  </si>
+  <si>
+    <t>Redirect Apms NUI (Registered checkout)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -157,12 +187,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Futura Next"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -178,15 +202,22 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF333333"/>
       <name val="Arial Nova"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial Nova"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Arial Nova"/>
       <family val="2"/>
     </font>
@@ -206,12 +237,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="5" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -234,23 +265,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="5"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="5"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="5"/>
+      </right>
+      <top style="thin">
+        <color theme="5"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -565,14 +634,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD4B857-567B-43E4-94E9-E00C544380EB}">
-  <dimension ref="B2:C38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="58.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="58.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1" customWidth="1"/>
     <col min="2" max="3" width="58.85546875" style="1"/>
@@ -580,295 +649,548 @@
     <col min="44" max="16384" width="58.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="5"/>
     </row>
     <row r="4" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>36</v>
+      <c r="B4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>6</v>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>1</v>
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>33</v>
+      <c r="B7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>2</v>
+      <c r="B8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>3</v>
+      <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>4</v>
+      <c r="B10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>5</v>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>9</v>
+      <c r="B12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>34</v>
+      <c r="B13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="7" t="s">
+    </row>
+    <row r="19" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B14:C14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C33"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="58.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1" customWidth="1"/>
+    <col min="2" max="3" width="58.85546875" style="1"/>
+    <col min="4" max="43" width="9.7109375" style="1" customWidth="1"/>
+    <col min="44" max="16384" width="58.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="4" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="7" t="s">
+    <row r="19" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="8" t="s">
+      <c r="C29" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C30" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
+    <row r="31" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C31" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
+    <row r="32" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C32" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="8" t="s">
+    <row r="33" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C33" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>